<commit_message>
another_source, lib_files, lib_photos ...
</commit_message>
<xml_diff>
--- a/Astrology/Moon/Eclipt/moon_comparison.xlsx
+++ b/Astrology/Moon/Eclipt/moon_comparison.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -752,6 +752,80 @@
         <v>7.599</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>2024-12-10 22:53:53</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>28.895</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>19.413</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>1.414</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>364124.18</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>366798.3</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0.8108</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>0.7528</v>
+      </c>
+      <c r="J8" s="6" t="n">
+        <v>10.536</v>
+      </c>
+      <c r="K8" s="6" t="n">
+        <v>9.866</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t>2024-12-11 21:31:15</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>42.614</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>33.039</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>3.313</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>2.516</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>365226.46</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>365639.93</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0.8898</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>0.8409</v>
+      </c>
+      <c r="J9" s="6" t="n">
+        <v>11.585</v>
+      </c>
+      <c r="K9" s="6" t="n">
+        <v>10.901</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>